<commit_message>
Informe previo - simulación 5
</commit_message>
<xml_diff>
--- a/5. COMPENSADORES/INFORME PREVIO/calculo_compensador.xlsx
+++ b/5. COMPENSADORES/INFORME PREVIO/calculo_compensador.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bremdows\UNSAAC\SEMESTRE VIII\lab-control-i\5. COMPENSADORES\INFORME PREVIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7622D9-968F-47E7-924C-46A8982A661A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA8E7FC-E290-43AE-A136-9E675CC296A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="456" windowWidth="11520" windowHeight="12504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="72" yWindow="1092" windowWidth="11508" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="subamortiguado" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -135,6 +135,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,7 +419,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -433,20 +434,20 @@
         <v>8</v>
       </c>
       <c r="B1">
-        <v>1.25</v>
+        <v>1.2450000000000001</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E1">
-        <v>3.0000000000000001E-3</v>
+        <v>1.1999999999999999E-6</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H1">
         <f>(0.0792*0.5086*1.36)/(B1*E1)</f>
-        <v>14.608619520000005</v>
+        <v>36668.221686746998</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -460,7 +461,7 @@
         <v>9</v>
       </c>
       <c r="E2">
-        <v>180</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -469,14 +470,14 @@
       </c>
       <c r="B3">
         <f>1/(B7*C7)</f>
-        <v>12.5</v>
+        <v>12.450000000000003</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E3">
         <f>1/((D7+E7)*F7)</f>
-        <v>0.54</v>
+        <v>1.9199999999999998E-4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -520,11 +521,11 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>B7*($B$1-1)</f>
-        <v>20000</v>
+        <v>19678.714859437758</v>
       </c>
       <c r="B7">
         <f>1/($B$2*$B$1*C7)</f>
-        <v>80000</v>
+        <v>80321.285140562235</v>
       </c>
       <c r="C7">
         <f>1*10^-6</f>
@@ -532,11 +533,11 @@
       </c>
       <c r="D7">
         <f>1/($E$2*F7)</f>
-        <v>5555.5555555555557</v>
+        <v>6250.0000000000009</v>
       </c>
       <c r="E7">
         <f>-(D7*($E$1-1))/($E$1)</f>
-        <v>1846296.2962962962</v>
+        <v>5208327083.333334</v>
       </c>
       <c r="F7">
         <f>1*10^-6</f>
@@ -547,17 +548,17 @@
       </c>
       <c r="H7">
         <f>G7*$H$1</f>
-        <v>1460.8619520000004</v>
+        <v>3666822.1686747</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" ref="A8:A14" si="0">B8*($B$1-1)</f>
-        <v>4255.3191489361707</v>
+        <v>4186.9606083910121</v>
       </c>
       <c r="B8">
         <f t="shared" ref="B8:B14" si="1">1/($B$2*$B$1*C8)</f>
-        <v>17021.276595744683</v>
+        <v>17089.635136289839</v>
       </c>
       <c r="C8">
         <f>4.7*10^-6</f>
@@ -565,11 +566,11 @@
       </c>
       <c r="D8">
         <f t="shared" ref="D8:D14" si="2">1/($E$2*F8)</f>
-        <v>1182.0330969267141</v>
+        <v>1329.7872340425533</v>
       </c>
       <c r="E8">
         <f t="shared" ref="E8:E14" si="3">-(D8*($E$1-1))/($E$1)</f>
-        <v>392828.99921197793</v>
+        <v>1108154698.5815606</v>
       </c>
       <c r="F8">
         <f>4.7*10^-6</f>
@@ -580,29 +581,29 @@
       </c>
       <c r="H8">
         <f t="shared" ref="H8:H18" si="4">G8*$H$1</f>
-        <v>1753.0343424000007</v>
+        <v>4400186.6024096394</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="1">
         <f t="shared" si="0"/>
-        <v>2000</v>
-      </c>
-      <c r="B9">
+        <v>1967.8714859437762</v>
+      </c>
+      <c r="B9" s="1">
         <f t="shared" si="1"/>
-        <v>8000</v>
-      </c>
-      <c r="C9">
+        <v>8032.1285140562259</v>
+      </c>
+      <c r="C9" s="1">
         <f>10*10^-6</f>
         <v>9.9999999999999991E-6</v>
       </c>
       <c r="D9">
         <f t="shared" si="2"/>
-        <v>555.55555555555554</v>
+        <v>625</v>
       </c>
       <c r="E9">
         <f t="shared" si="3"/>
-        <v>184629.62962962964</v>
+        <v>520832708.33333331</v>
       </c>
       <c r="F9">
         <f>10*10^-6</f>
@@ -613,17 +614,17 @@
       </c>
       <c r="H9" s="1">
         <f t="shared" si="4"/>
-        <v>2191.2929280000008</v>
+        <v>5500233.2530120499</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>909.09090909090901</v>
+        <v>894.48703906535275</v>
       </c>
       <c r="B10">
         <f t="shared" si="1"/>
-        <v>3636.363636363636</v>
+        <v>3650.9675063891932</v>
       </c>
       <c r="C10">
         <f>22*10^-6</f>
@@ -631,11 +632,11 @@
       </c>
       <c r="D10" s="1">
         <f t="shared" si="2"/>
-        <v>252.52525252525254</v>
+        <v>284.09090909090912</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="3"/>
-        <v>83922.558922558921</v>
+        <v>236742140.15151516</v>
       </c>
       <c r="F10" s="1">
         <f>22*10^-6</f>
@@ -646,17 +647,17 @@
       </c>
       <c r="H10" s="1">
         <f t="shared" si="4"/>
-        <v>3213.8962944000009</v>
+        <v>8067008.7710843394</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
-        <v>425.53191489361706</v>
+        <v>418.69606083910122</v>
       </c>
       <c r="B11">
         <f t="shared" si="1"/>
-        <v>1702.1276595744682</v>
+        <v>1708.9635136289839</v>
       </c>
       <c r="C11">
         <f>47*10^-6</f>
@@ -664,11 +665,11 @@
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>118.20330969267141</v>
+        <v>132.97872340425533</v>
       </c>
       <c r="E11">
-        <f t="shared" si="3"/>
-        <v>39282.899921197801</v>
+        <f>-(D11*($E$1-1))/($E$1)</f>
+        <v>110815469.85815604</v>
       </c>
       <c r="F11">
         <f>47*10^-6</f>
@@ -679,29 +680,29 @@
       </c>
       <c r="H11">
         <f t="shared" si="4"/>
-        <v>4820.844441600002</v>
+        <v>12100513.15662651</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+      <c r="A12" s="4">
         <f t="shared" si="0"/>
-        <v>200.00000000000003</v>
-      </c>
-      <c r="B12" s="1">
+        <v>196.78714859437758</v>
+      </c>
+      <c r="B12" s="4">
         <f t="shared" si="1"/>
-        <v>800.00000000000011</v>
-      </c>
-      <c r="C12" s="1">
+        <v>803.21285140562247</v>
+      </c>
+      <c r="C12" s="4">
         <f>100*10^-6</f>
         <v>9.9999999999999991E-5</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>55.555555555555557</v>
+        <v>62.5</v>
       </c>
       <c r="E12">
         <f t="shared" si="3"/>
-        <v>18462.962962962964</v>
+        <v>52083270.833333336</v>
       </c>
       <c r="F12">
         <f>100*10^-6</f>
@@ -712,17 +713,17 @@
       </c>
       <c r="H12">
         <f t="shared" si="4"/>
-        <v>6866.0511744000023</v>
+        <v>17234064.192771088</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
-        <v>42.553191489361701</v>
+        <v>41.869606083910128</v>
       </c>
       <c r="B13">
         <f t="shared" si="1"/>
-        <v>170.21276595744681</v>
+        <v>170.8963513628984</v>
       </c>
       <c r="C13">
         <f>470*10^-6</f>
@@ -730,11 +731,11 @@
       </c>
       <c r="D13">
         <f t="shared" si="2"/>
-        <v>11.82033096926714</v>
+        <v>13.297872340425531</v>
       </c>
       <c r="E13">
         <f t="shared" si="3"/>
-        <v>3928.2899921197795</v>
+        <v>11081546.985815601</v>
       </c>
       <c r="F13">
         <f>470*10^-6</f>
@@ -748,11 +749,11 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19.678714859437758</v>
       </c>
       <c r="B14">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>80.321285140562239</v>
       </c>
       <c r="C14">
         <f>1000*10^-6</f>
@@ -760,11 +761,11 @@
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>5.5555555555555554</v>
+        <v>6.25</v>
       </c>
       <c r="E14">
         <f t="shared" si="3"/>
-        <v>1846.2962962962963</v>
+        <v>5208327.083333333</v>
       </c>
       <c r="F14">
         <f>1000*10^-6</f>

</xml_diff>

<commit_message>
Implementacion - lab. 5 sub - finalizada
</commit_message>
<xml_diff>
--- a/5. COMPENSADORES/INFORME PREVIO/calculo_compensador.xlsx
+++ b/5. COMPENSADORES/INFORME PREVIO/calculo_compensador.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bremdows\UNSAAC\SEMESTRE VIII\lab-control-i\5. COMPENSADORES\INFORME PREVIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA8E7FC-E290-43AE-A136-9E675CC296A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDC8DAD-6680-4763-82A1-1A9251FE1D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72" yWindow="1092" windowWidth="11508" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="456" windowWidth="11520" windowHeight="12504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="subamortiguado" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>R5</t>
   </si>
@@ -67,15 +67,9 @@
     <t>Cero</t>
   </si>
   <si>
-    <t>Krtr</t>
-  </si>
-  <si>
     <t>Polo</t>
   </si>
   <si>
-    <t>Kc</t>
-  </si>
-  <si>
     <t>R9</t>
   </si>
   <si>
@@ -83,6 +77,15 @@
   </si>
   <si>
     <t>|</t>
+  </si>
+  <si>
+    <t>Kat</t>
+  </si>
+  <si>
+    <t>kt</t>
+  </si>
+  <si>
+    <t>Ganancia</t>
   </si>
 </sst>
 </file>
@@ -114,9 +117,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -126,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -136,6 +148,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,20 +465,20 @@
         <v>8</v>
       </c>
       <c r="B1">
-        <v>1.2450000000000001</v>
+        <v>1.9709000000000001</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E1">
-        <v>1.1999999999999999E-6</v>
+        <v>1.3019000000000001</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H1">
-        <f>(0.0792*0.5086*1.36)/(B1*E1)</f>
-        <v>36668.221686746998</v>
+        <f>E1*B1</f>
+        <v>2.5659147100000004</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -461,23 +492,21 @@
         <v>9</v>
       </c>
       <c r="E2">
-        <v>160</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <f>1/(B7*C7)</f>
-        <v>12.450000000000003</v>
+        <v>43.36</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <f>1/((D7+E7)*F7)</f>
-        <v>1.9199999999999998E-4</v>
+        <v>0.1148</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -486,11 +515,15 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -502,314 +535,294 @@
       <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>13</v>
+      <c r="G6" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f>B7*($B$1-1)</f>
-        <v>19678.714859437758</v>
+        <f>((1/$B$2)-B7*C7)/(C7)</f>
+        <v>76937.269372693743</v>
       </c>
       <c r="B7">
-        <f>1/($B$2*$B$1*C7)</f>
-        <v>80321.285140562235</v>
+        <f>(1)/($B$3*C7)</f>
+        <v>23062.730627306275</v>
       </c>
       <c r="C7">
         <f>1*10^-6</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="12">
         <f>1/($E$2*F7)</f>
-        <v>6250.0000000000009</v>
+        <v>40000</v>
       </c>
       <c r="E7">
-        <f>-(D7*($E$1-1))/($E$1)</f>
-        <v>5208327083.333334</v>
-      </c>
-      <c r="F7">
+        <f>((1/$E$3) - D7*F7)/(F7)</f>
+        <v>8670801.3937282246</v>
+      </c>
+      <c r="F7" s="6">
         <f>1*10^-6</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="G7">
-        <v>100</v>
+      <c r="G7" s="12">
+        <v>3300</v>
       </c>
       <c r="H7">
-        <f>G7*$H$1</f>
-        <v>3666822.1686747</v>
+        <f>($H$1*A7*B7*G7*(D7+E7))/(D7*E7*(A7+B7))</f>
+        <v>3773.4841761743446</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" ref="A8:A14" si="0">B8*($B$1-1)</f>
-        <v>4186.9606083910121</v>
+        <f t="shared" ref="A8:A14" si="0">((1/$B$2)-B8*C8)/(C8)</f>
+        <v>16369.631781424201</v>
       </c>
       <c r="B8">
-        <f t="shared" ref="B8:B14" si="1">1/($B$2*$B$1*C8)</f>
-        <v>17089.635136289839</v>
+        <f t="shared" ref="B8:B14" si="1">1/($B$3*C8)</f>
+        <v>4906.9639632566541</v>
       </c>
       <c r="C8">
         <f>4.7*10^-6</f>
         <v>4.6999999999999999E-6</v>
       </c>
-      <c r="D8">
-        <f t="shared" ref="D8:D14" si="2">1/($E$2*F8)</f>
-        <v>1329.7872340425533</v>
+      <c r="D8" s="12">
+        <f>1/($E$2*F8)</f>
+        <v>8510.6382978723414</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8:E14" si="3">-(D8*($E$1-1))/($E$1)</f>
-        <v>1108154698.5815606</v>
-      </c>
-      <c r="F8">
+        <f>((1/$E$3)-D8*F8)/(F8)</f>
+        <v>1844851.3603677072</v>
+      </c>
+      <c r="F8" s="6">
         <f>4.7*10^-6</f>
         <v>4.6999999999999999E-6</v>
       </c>
-      <c r="G8">
-        <v>120</v>
+      <c r="G8" s="12">
+        <v>3900</v>
       </c>
       <c r="H8">
-        <f t="shared" ref="H8:H18" si="4">G8*$H$1</f>
-        <v>4400186.6024096394</v>
+        <f t="shared" ref="H8:H14" si="2">($H$1*A8*B8*G8*(D8+E8))/(D8*E8*(A8+B8))</f>
+        <v>4459.5722082060429</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+      <c r="A9" s="4">
         <f t="shared" si="0"/>
-        <v>1967.8714859437762</v>
-      </c>
-      <c r="B9" s="1">
+        <v>7693.7269372693745</v>
+      </c>
+      <c r="B9" s="4">
         <f t="shared" si="1"/>
-        <v>8032.1285140562259</v>
-      </c>
-      <c r="C9" s="1">
+        <v>2306.2730627306273</v>
+      </c>
+      <c r="C9" s="4">
         <f>10*10^-6</f>
         <v>9.9999999999999991E-6</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="2"/>
-        <v>625</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="3"/>
-        <v>520832708.33333331</v>
-      </c>
-      <c r="F9">
+      <c r="D9" s="13">
+        <f>1/($E$2*F9)</f>
+        <v>4000</v>
+      </c>
+      <c r="E9" s="4">
+        <f>((1/$E$3)-D9*F9)/(F9)</f>
+        <v>867080.13937282248</v>
+      </c>
+      <c r="F9" s="8">
         <f>10*10^-6</f>
         <v>9.9999999999999991E-6</v>
       </c>
-      <c r="G9" s="1">
-        <v>150</v>
-      </c>
-      <c r="H9" s="1">
-        <f t="shared" si="4"/>
-        <v>5500233.2530120499</v>
+      <c r="G9" s="13">
+        <v>4700</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>5374.3562509149751</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>894.48703906535275</v>
+        <v>3497.1486078497155</v>
       </c>
       <c r="B10">
         <f t="shared" si="1"/>
-        <v>3650.9675063891932</v>
+        <v>1048.3059376048307</v>
       </c>
       <c r="C10">
         <f>22*10^-6</f>
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="D10" s="1">
-        <f t="shared" si="2"/>
-        <v>284.09090909090912</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" si="3"/>
-        <v>236742140.15151516</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="D10" s="12">
+        <f>1/($E$2*F10)</f>
+        <v>1818.181818181818</v>
+      </c>
+      <c r="E10">
+        <f>((1/$E$3)-D10*F10)/(F10)</f>
+        <v>394127.33607855567</v>
+      </c>
+      <c r="F10" s="8">
         <f>22*10^-6</f>
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="G10" s="1">
-        <v>220</v>
-      </c>
-      <c r="H10" s="1">
-        <f t="shared" si="4"/>
-        <v>8067008.7710843394</v>
+      <c r="G10" s="13">
+        <v>6800</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>7775.6643630259205</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>418.69606083910122</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="1"/>
-        <v>1708.9635136289839</v>
-      </c>
-      <c r="C11">
+      <c r="A11" s="1">
+        <f>((1/$B$2)-B11*C11)/(C11)</f>
+        <v>1636.96317814242</v>
+      </c>
+      <c r="B11" s="1">
+        <f>1/($B$3*C11)</f>
+        <v>490.69639632566538</v>
+      </c>
+      <c r="C11" s="1">
         <f>47*10^-6</f>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="2"/>
-        <v>132.97872340425533</v>
-      </c>
-      <c r="E11">
-        <f>-(D11*($E$1-1))/($E$1)</f>
-        <v>110815469.85815604</v>
-      </c>
-      <c r="F11">
+      <c r="D11" s="15">
+        <f>1/($E$2*F11)</f>
+        <v>851.06382978723411</v>
+      </c>
+      <c r="E11" s="1">
+        <f>((1/$E$3)-D11*F11)/(F11)</f>
+        <v>184485.13603677074</v>
+      </c>
+      <c r="F11" s="7">
         <f>47*10^-6</f>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="G11">
-        <v>330</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="4"/>
-        <v>12100513.15662651</v>
+      <c r="G11" s="15">
+        <v>470</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="2"/>
+        <v>537.4356250914974</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+      <c r="A12">
         <f t="shared" si="0"/>
-        <v>196.78714859437758</v>
-      </c>
-      <c r="B12" s="4">
+        <v>769.37269372693743</v>
+      </c>
+      <c r="B12">
         <f t="shared" si="1"/>
-        <v>803.21285140562247</v>
-      </c>
-      <c r="C12" s="4">
+        <v>230.62730627306274</v>
+      </c>
+      <c r="C12">
         <f>100*10^-6</f>
         <v>9.9999999999999991E-5</v>
       </c>
-      <c r="D12">
-        <f t="shared" si="2"/>
-        <v>62.5</v>
+      <c r="D12" s="12">
+        <f>1/($E$2*F12)</f>
+        <v>400.00000000000006</v>
       </c>
       <c r="E12">
-        <f t="shared" si="3"/>
-        <v>52083270.833333336</v>
-      </c>
-      <c r="F12">
+        <f>((1/$E$3)-D12*F12)/(F12)</f>
+        <v>86708.013937282245</v>
+      </c>
+      <c r="F12" s="6">
         <f>100*10^-6</f>
         <v>9.9999999999999991E-5</v>
       </c>
-      <c r="G12">
-        <v>470</v>
+      <c r="G12" s="12">
+        <v>10000</v>
       </c>
       <c r="H12">
-        <f t="shared" si="4"/>
-        <v>17234064.192771088</v>
+        <f t="shared" si="2"/>
+        <v>11434.800533861648</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
-        <v>41.869606083910128</v>
+        <v>163.69631781424201</v>
       </c>
       <c r="B13">
         <f t="shared" si="1"/>
-        <v>170.8963513628984</v>
+        <v>49.069639632566535</v>
       </c>
       <c r="C13">
         <f>470*10^-6</f>
         <v>4.6999999999999999E-4</v>
       </c>
-      <c r="D13">
-        <f t="shared" si="2"/>
-        <v>13.297872340425531</v>
+      <c r="D13" s="12">
+        <f>1/($E$2*F13)</f>
+        <v>85.106382978723403</v>
       </c>
       <c r="E13">
-        <f t="shared" si="3"/>
-        <v>11081546.985815601</v>
-      </c>
-      <c r="F13">
+        <f>((1/$E$3)-D13*F13)/(F13)</f>
+        <v>18448.513603677075</v>
+      </c>
+      <c r="F13" s="6">
         <f>470*10^-6</f>
         <v>4.6999999999999999E-4</v>
       </c>
+      <c r="G13" s="12">
+        <v>560</v>
+      </c>
       <c r="H13">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>640.34882989625225</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>19.678714859437758</v>
+        <v>76.937269372693734</v>
       </c>
       <c r="B14">
         <f t="shared" si="1"/>
-        <v>80.321285140562239</v>
+        <v>23.062730627306273</v>
       </c>
       <c r="C14">
         <f>1000*10^-6</f>
         <v>1E-3</v>
       </c>
-      <c r="D14">
-        <f t="shared" si="2"/>
-        <v>6.25</v>
+      <c r="D14" s="12">
+        <f t="shared" ref="D8:D14" si="3">1/($E$2*F14)</f>
+        <v>40</v>
       </c>
       <c r="E14">
-        <f t="shared" si="3"/>
-        <v>5208327.083333333</v>
-      </c>
-      <c r="F14">
+        <f>((1/$E$3)-D14*F14)/(F14)</f>
+        <v>8670.8013937282249</v>
+      </c>
+      <c r="F14" s="6">
         <f>1000*10^-6</f>
         <v>1E-3</v>
       </c>
+      <c r="G14" s="12">
+        <v>1200</v>
+      </c>
       <c r="H14">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>1372.1760640633977</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H15">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H19">
-        <f>G19*$H$1</f>
-        <v>0</v>
-      </c>
+      <c r="G15" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -820,7 +833,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H15" sqref="H15:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -830,20 +843,20 @@
         <v>8</v>
       </c>
       <c r="B1">
-        <v>1.1000000000000001</v>
+        <v>1.9709000000000001</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E1">
-        <v>4.0000000000000001E-3</v>
+        <v>1.3019000000000001</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H1">
-        <f>(0.609*1.1854*100)/(B1*E1)</f>
-        <v>16407.013636363634</v>
+        <f>E1*B1</f>
+        <v>2.5659147100000004</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -851,29 +864,27 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>190</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E2">
-        <v>5.5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <f>1/(B7*C7)</f>
-        <v>209.00000000000006</v>
+        <v>43.36</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <f>1/((D7+E7)*F7)</f>
-        <v>2.2000000000000002E-2</v>
+        <v>0.1148</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -882,11 +893,12 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -898,298 +910,289 @@
       <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>13</v>
+      <c r="G6" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <f>B7*($B$1-1)</f>
-        <v>478.46889952153145</v>
-      </c>
-      <c r="B7" s="1">
-        <f>1/($B$2*$B$1*C7)</f>
-        <v>4784.6889952153106</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="A7">
+        <f>((1/$B$2)-B7*C7)/(C7)</f>
+        <v>76937.269372693743</v>
+      </c>
+      <c r="B7">
+        <f>1/($B$3*C7)</f>
+        <v>23062.730627306275</v>
+      </c>
+      <c r="C7">
         <f>1*10^-6</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="12">
         <f>1/($E$2*F7)</f>
-        <v>181818.18181818182</v>
+        <v>40000</v>
       </c>
       <c r="E7">
-        <f>-(D7*($E$1-1))/($E$1)</f>
-        <v>45272727.272727273</v>
-      </c>
-      <c r="F7">
+        <f>((1/$E$3)-D7*F7)/(F7)</f>
+        <v>8670801.3937282246</v>
+      </c>
+      <c r="F7" s="6">
         <f>1*10^-6</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="G7" s="1">
-        <v>100</v>
-      </c>
-      <c r="H7" s="1">
-        <f>G7*$H$1</f>
-        <v>1640701.3636363633</v>
+      <c r="G7" s="12">
+        <v>3300</v>
+      </c>
+      <c r="H7">
+        <f>$H$1*A7*G7/E7</f>
+        <v>75.133511365199851</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <f t="shared" ref="A8:A14" si="0">B8*($B$1-1)</f>
-        <v>101.80189351521946</v>
-      </c>
-      <c r="B8" s="1">
-        <f t="shared" ref="B8:B14" si="1">1/($B$2*$B$1*C8)</f>
-        <v>1018.0189351521936</v>
-      </c>
-      <c r="C8" s="1">
+      <c r="A8">
+        <f t="shared" ref="A8:A14" si="0">((1/$B$2)-B8*C8)/(C8)</f>
+        <v>16369.631781424201</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ref="B8:B14" si="1">1/($B$3*C8)</f>
+        <v>4906.9639632566541</v>
+      </c>
+      <c r="C8">
         <f>4.7*10^-6</f>
         <v>4.6999999999999999E-6</v>
       </c>
-      <c r="D8">
-        <f t="shared" ref="D8:D14" si="2">1/($E$2*F8)</f>
-        <v>38684.71953578337</v>
+      <c r="D8" s="12">
+        <f>1/($E$2*F8)</f>
+        <v>8510.6382978723414</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8:E14" si="3">-(D8*($E$1-1))/($E$1)</f>
-        <v>9632495.1644100584</v>
-      </c>
-      <c r="F8">
+        <f t="shared" ref="E8:E14" si="2">((1/$E$3)-D8*F8)/(F8)</f>
+        <v>1844851.3603677072</v>
+      </c>
+      <c r="F8" s="6">
         <f>4.7*10^-6</f>
         <v>4.6999999999999999E-6</v>
       </c>
+      <c r="G8" s="12">
+        <v>3900</v>
+      </c>
       <c r="H8">
-        <f t="shared" ref="H8:H18" si="4">G8*$H$1</f>
-        <v>0</v>
+        <f t="shared" ref="H8:H14" si="3">$H$1*A8*G8/E8</f>
+        <v>88.794149795236194</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="4">
         <f t="shared" si="0"/>
-        <v>47.846889952153148</v>
-      </c>
-      <c r="B9">
+        <v>7693.7269372693745</v>
+      </c>
+      <c r="B9" s="4">
         <f t="shared" si="1"/>
-        <v>478.46889952153106</v>
-      </c>
-      <c r="C9">
+        <v>2306.2730627306273</v>
+      </c>
+      <c r="C9" s="4">
         <f>10*10^-6</f>
         <v>9.9999999999999991E-6</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="13">
+        <f>1/($E$2*F9)</f>
+        <v>4000</v>
+      </c>
+      <c r="E9" s="4">
         <f t="shared" si="2"/>
-        <v>18181.818181818184</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="3"/>
-        <v>4527272.7272727275</v>
-      </c>
-      <c r="F9">
+        <v>867080.13937282248</v>
+      </c>
+      <c r="F9" s="8">
         <f>10*10^-6</f>
         <v>9.9999999999999991E-6</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="4"/>
-        <v>0</v>
+      <c r="G9" s="13">
+        <v>4700</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="3"/>
+        <v>107.00833436861798</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>21.748586341887794</v>
+        <v>3497.1486078497155</v>
       </c>
       <c r="B10">
         <f t="shared" si="1"/>
-        <v>217.48586341887776</v>
+        <v>1048.3059376048307</v>
       </c>
       <c r="C10">
         <f>22*10^-6</f>
         <v>2.1999999999999999E-5</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="12">
+        <f>1/($E$2*F10)</f>
+        <v>1818.181818181818</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="2"/>
-        <v>8264.4628099173551</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="3"/>
-        <v>2057851.2396694212</v>
-      </c>
-      <c r="F10">
+        <v>394127.33607855567</v>
+      </c>
+      <c r="F10" s="8">
         <f>22*10^-6</f>
         <v>2.1999999999999999E-5</v>
       </c>
+      <c r="G10" s="13">
+        <v>6800</v>
+      </c>
       <c r="H10">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>154.82056887374517</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
-        <v>10.180189351521946</v>
+        <v>1636.96317814242</v>
       </c>
       <c r="B11">
         <f t="shared" si="1"/>
-        <v>101.80189351521938</v>
+        <v>490.69639632566538</v>
       </c>
       <c r="C11">
         <f>47*10^-6</f>
         <v>4.6999999999999997E-5</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="12">
+        <f>1/($E$2*F11)</f>
+        <v>851.06382978723411</v>
+      </c>
+      <c r="E11">
         <f t="shared" si="2"/>
-        <v>3868.4719535783365</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="3"/>
-        <v>963249.51644100575</v>
-      </c>
-      <c r="F11">
+        <v>184485.13603677074</v>
+      </c>
+      <c r="F11" s="6">
         <f>47*10^-6</f>
         <v>4.6999999999999997E-5</v>
       </c>
+      <c r="G11" s="12">
+        <v>330</v>
+      </c>
       <c r="H11">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>7.5133511365199857</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
-        <v>4.7846889952153147</v>
+        <v>769.37269372693743</v>
       </c>
       <c r="B12">
         <f t="shared" si="1"/>
-        <v>47.846889952153106</v>
+        <v>230.62730627306274</v>
       </c>
       <c r="C12">
         <f>100*10^-6</f>
         <v>9.9999999999999991E-5</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="12">
+        <f>1/($E$2*F12)</f>
+        <v>400.00000000000006</v>
+      </c>
+      <c r="E12">
         <f t="shared" si="2"/>
-        <v>1818.1818181818185</v>
-      </c>
-      <c r="E12">
-        <f>-(D12*($E$1-1))/($E$1)</f>
-        <v>452727.27272727282</v>
-      </c>
-      <c r="F12">
+        <v>86708.013937282245</v>
+      </c>
+      <c r="F12" s="6">
         <f>100*10^-6</f>
         <v>9.9999999999999991E-5</v>
       </c>
+      <c r="G12" s="12">
+        <v>470</v>
+      </c>
       <c r="H12">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>10.700833436861798</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
-        <v>1.0180189351521947</v>
+        <v>163.69631781424201</v>
       </c>
       <c r="B13">
         <f t="shared" si="1"/>
-        <v>10.180189351521937</v>
+        <v>49.069639632566535</v>
       </c>
       <c r="C13">
         <f>470*10^-6</f>
         <v>4.6999999999999999E-4</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="12">
+        <f>1/($E$2*F13)</f>
+        <v>85.106382978723403</v>
+      </c>
+      <c r="E13">
         <f t="shared" si="2"/>
-        <v>386.84719535783364</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="3"/>
-        <v>96324.951644100584</v>
-      </c>
-      <c r="F13">
+        <v>18448.513603677075</v>
+      </c>
+      <c r="F13" s="6">
         <f>470*10^-6</f>
         <v>4.6999999999999999E-4</v>
       </c>
+      <c r="G13" s="12">
+        <v>560</v>
+      </c>
       <c r="H13">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>12.74992920136725</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>0.47846889952153143</v>
+        <v>76.937269372693734</v>
       </c>
       <c r="B14">
         <f t="shared" si="1"/>
-        <v>4.7846889952153102</v>
+        <v>23.062730627306273</v>
       </c>
       <c r="C14">
         <f>1000*10^-6</f>
         <v>1E-3</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="12">
+        <f t="shared" ref="D14" si="4">1/($E$2*F14)</f>
+        <v>40</v>
+      </c>
+      <c r="E14">
         <f t="shared" si="2"/>
-        <v>181.81818181818184</v>
-      </c>
-      <c r="E14" s="1">
-        <f t="shared" si="3"/>
-        <v>45272.727272727279</v>
-      </c>
-      <c r="F14" s="1">
+        <v>8670.8013937282249</v>
+      </c>
+      <c r="F14" s="6">
         <f>1000*10^-6</f>
         <v>1E-3</v>
       </c>
+      <c r="G14" s="12">
+        <v>1200</v>
+      </c>
       <c r="H14">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H15">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="H17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="H18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="H19">
-        <f>G19*$H$1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>27.321276860072672</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Informe final 5 - 6 finalizado
</commit_message>
<xml_diff>
--- a/5. COMPENSADORES/INFORME PREVIO/calculo_compensador.xlsx
+++ b/5. COMPENSADORES/INFORME PREVIO/calculo_compensador.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNSAAC\SEMESTRE VIII\lab-control-i\5. COMPENSADORES\INFORME PREVIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76B7A02-6A02-4BB9-A11B-C32EF82DF079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F710EA50-4EAC-4834-95F9-CD8FF7CE53AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14865" yWindow="0" windowWidth="13935" windowHeight="16200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="13935" windowHeight="16200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="subamortiguado" sheetId="1" r:id="rId1"/>
@@ -138,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -155,7 +155,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,7 +438,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,15 +818,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE6816B4-834C-4C8E-B4C6-41F500A21A8A}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -848,7 +847,7 @@
         <v>10.8843677</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -862,7 +861,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -876,7 +875,7 @@
         <v>0.51119999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
@@ -892,7 +891,7 @@
       </c>
       <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -918,7 +917,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>((1/$B$2)-B7*C7)/(C7)</f>
         <v>15302.979515677542</v>
@@ -951,7 +950,7 @@
         <v>3405.6259903155274</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ref="A8:A14" si="1">((1/$B$2)-B8*C8)/(C8)</f>
         <v>3255.9530884420301</v>
@@ -984,7 +983,7 @@
         <v>4024.8307158274411</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>1530.2979515677541</v>
@@ -1017,7 +1016,7 @@
         <v>4850.4370165099945</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>695.58997798534278</v>
@@ -1050,7 +1049,7 @@
         <v>7017.6535558016913</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>((1/$B$2)-B11*C11)/(C11)</f>
         <v>325.59530884420298</v>
@@ -1082,9 +1081,8 @@
         <f t="shared" si="4"/>
         <v>4850.4370165099945</v>
       </c>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>153.02979515677541</v>
@@ -1117,7 +1115,7 @@
         <v>4850.4370165099936</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>32.559530884420298</v>
@@ -1150,7 +1148,7 @@
         <v>122.96264052718857</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>15.302979515677539</v>

</xml_diff>